<commit_message>
dsa hashing and linked lists
</commit_message>
<xml_diff>
--- a/java/TopInterview150_LC75.xlsx
+++ b/java/TopInterview150_LC75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7436521-DA41-4B32-BCA0-BD94879F2D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F88BACC-B83D-4DD9-8268-F3EB78766846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="106">
   <si>
     <t>Question</t>
   </si>
@@ -336,6 +336,24 @@
   </si>
   <si>
     <t xml:space="preserve">https://leetcode.com/problems/n-th-tribonacci-number/solutions/4182906/easy-and-understandable-solution-beets-100-percents-user/?envType=study-plan-v2&amp;envId=leetcode-75 </t>
+  </si>
+  <si>
+    <t>2215. Find the Difference of Two Arrays</t>
+  </si>
+  <si>
+    <t>Symmetric Difference with HashSets. Create and populate Hashlists, convert to ArrayLists, then use removeAll() method to find the symmetric difference.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/find-the-difference-of-two-arrays/solutions/4390106/97-beats-only-using-hashset-friendly/?envType=study-plan-v2&amp;envId=leetcode-75 </t>
+  </si>
+  <si>
+    <t>2095. Delete the Middle Node of a Linked List</t>
+  </si>
+  <si>
+    <t>1st pass to find the length, calculate the mid point, then traverse and connect prev.next to prev.next.next, or to slow to fast, skipping the nth node.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/delete-the-middle-node-of-a-linked-list/solutions/4335889/100-best-approach-slow-fast-pointers/?envType=study-plan-v2&amp;envId=leetcode-75 </t>
   </si>
 </sst>
 </file>
@@ -687,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1158,6 +1176,40 @@
       </c>
       <c r="E27" s="2" t="s">
         <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" t="s">
+        <v>101</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" t="s">
+        <v>104</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1188,6 +1240,8 @@
     <hyperlink ref="E25" r:id="rId24" xr:uid="{ACAEC1CD-10DF-4856-8EC9-B5984A41BBD9}"/>
     <hyperlink ref="E26" r:id="rId25" xr:uid="{0D9AE99D-BD2B-492B-9FF7-59E76EF291AF}"/>
     <hyperlink ref="E27" r:id="rId26" xr:uid="{98BF0048-C974-4034-8134-1C8055BB9AAA}"/>
+    <hyperlink ref="E28" r:id="rId27" xr:uid="{F27AD6A2-14B4-4663-BC6B-F7F546B8C3C0}"/>
+    <hyperlink ref="E29" r:id="rId28" xr:uid="{E51EAA8B-2613-4EAF-93A7-6D7A934EA177}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dsa divide and conquer
</commit_message>
<xml_diff>
--- a/java/TopInterview150_LC75.xlsx
+++ b/java/TopInterview150_LC75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82D3073-723A-4CD8-BB95-A81A777C5AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E09FBB-C8D2-4320-B088-7F9AE5BC3892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="126">
   <si>
     <t>Question</t>
   </si>
@@ -402,6 +402,18 @@
   </si>
   <si>
     <t xml:space="preserve">https://leetcode.com/problems/path-sum/solutions/3977919/easy-solution-python3-c-c-c-java-explain-line-by-line-with-image/?envType=study-plan-v2&amp;envId=top-interview-150 </t>
+  </si>
+  <si>
+    <t>427. Construct Quad Tree</t>
+  </si>
+  <si>
+    <t>Divide and Conquer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/construct-quad-tree/solutions/3234703/clean-codes-full-explanation-helper-method-c-java-python3/?envType=study-plan-v2&amp;envId=top-interview-150 </t>
+  </si>
+  <si>
+    <t>Straightforward OOP and grid recursion. Have a helper function and use a 2d loop to check if all values are the same. Use the same input grid and pointers to recursively call each subgrid.</t>
   </si>
 </sst>
 </file>
@@ -753,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1343,6 +1355,23 @@
       </c>
       <c r="E34" s="2" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>122</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>123</v>
+      </c>
+      <c r="D35" t="s">
+        <v>125</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1380,6 +1409,7 @@
     <hyperlink ref="E32" r:id="rId31" xr:uid="{3B7B87A5-78F0-4B00-BB35-0A2D4D761723}"/>
     <hyperlink ref="E33" r:id="rId32" xr:uid="{95DD2349-D931-4A03-BB97-5CD7303127E1}"/>
     <hyperlink ref="E34" r:id="rId33" xr:uid="{16963203-6A0F-4E0F-9FD3-132131942214}"/>
+    <hyperlink ref="E35" r:id="rId34" xr:uid="{2E7BF211-9A65-4432-8AC6-E305E5481B16}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dsa stacks and fcc web
</commit_message>
<xml_diff>
--- a/java/TopInterview150_LC75.xlsx
+++ b/java/TopInterview150_LC75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BA6E4D-75C0-43C2-A06F-2F433AA1F2A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8619111-B882-4066-A641-A12F7DD3B857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="132">
   <si>
     <t>Question</t>
   </si>
@@ -423,6 +423,15 @@
   </si>
   <si>
     <t xml:space="preserve">https://leetcode.com/problems/odd-even-linked-list/solutions/1606975/java-2-solutions-explanation-using-image-without-space/?envType=study-plan-v2&amp;envId=leetcode-75 </t>
+  </si>
+  <si>
+    <t>735. Asteroid Collision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/asteroid-collision/solutions/3394436/c-java-python-javascript-stack-with-explaination/?envType=study-plan-v2&amp;envId=leetcode-75 </t>
+  </si>
+  <si>
+    <t>The crux is to repeat the collision check at the top of the list. Just add to stack as you iterate the list, but consider the behavior for each case. Then at the end, populate the res list with the remaining stack elements.</t>
   </si>
 </sst>
 </file>
@@ -774,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1398,6 +1407,23 @@
       </c>
       <c r="E36" s="2" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>129</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" t="s">
+        <v>131</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1437,6 +1463,7 @@
     <hyperlink ref="E34" r:id="rId33" xr:uid="{16963203-6A0F-4E0F-9FD3-132131942214}"/>
     <hyperlink ref="E35" r:id="rId34" xr:uid="{2E7BF211-9A65-4432-8AC6-E305E5481B16}"/>
     <hyperlink ref="E36" r:id="rId35" xr:uid="{2C492EB7-7E6E-43F6-8E8C-97E2260B48DA}"/>
+    <hyperlink ref="E37" r:id="rId36" xr:uid="{7FA8BAF1-B262-4C59-8C55-18E8EBC381DE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dsa trees fcc web
</commit_message>
<xml_diff>
--- a/java/TopInterview150_LC75.xlsx
+++ b/java/TopInterview150_LC75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8619111-B882-4066-A641-A12F7DD3B857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46C8F7D-F596-4AAA-AD5F-08D57FB0481E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="135">
   <si>
     <t>Question</t>
   </si>
@@ -432,6 +432,15 @@
   </si>
   <si>
     <t>The crux is to repeat the collision check at the top of the list. Just add to stack as you iterate the list, but consider the behavior for each case. Then at the end, populate the res list with the remaining stack elements.</t>
+  </si>
+  <si>
+    <t>872. Leaf-Similar Trees</t>
+  </si>
+  <si>
+    <t>Create 2 lists, perform dfs on each root node and populate the lists with the leaf values. Then compare lists. You can use l1.equals(l2) instead of traversing the lists.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/leaf-similar-trees/solutions/2889643/easy-java-solution-using-recursion-and-arraylists-o-n/?envType=study-plan-v2&amp;envId=leetcode-75 </t>
   </si>
 </sst>
 </file>
@@ -783,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1424,6 +1433,23 @@
       </c>
       <c r="E37" s="2" t="s">
         <v>130</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>132</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" t="s">
+        <v>133</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1464,6 +1490,7 @@
     <hyperlink ref="E35" r:id="rId34" xr:uid="{2E7BF211-9A65-4432-8AC6-E305E5481B16}"/>
     <hyperlink ref="E36" r:id="rId35" xr:uid="{2C492EB7-7E6E-43F6-8E8C-97E2260B48DA}"/>
     <hyperlink ref="E37" r:id="rId36" xr:uid="{7FA8BAF1-B262-4C59-8C55-18E8EBC381DE}"/>
+    <hyperlink ref="E38" r:id="rId37" xr:uid="{E8445F29-8F3E-469F-8E84-916FDFC5CB09}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dsa greedy and web css
</commit_message>
<xml_diff>
--- a/java/TopInterview150_LC75.xlsx
+++ b/java/TopInterview150_LC75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02790A56-3695-4596-BC2C-8F2D97412A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0157FB-7B21-4595-B5FD-FC5E87ACFE5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="149">
   <si>
     <t>Question</t>
   </si>
@@ -465,6 +465,24 @@
   </si>
   <si>
     <t>Iterate with modulus and word length conditions. StringBuilder and while loops are optimal. You can just iterate i and do both conditions at once, without alternating the loop behavior.</t>
+  </si>
+  <si>
+    <t>1071. Greatest Common Divisor of Strings</t>
+  </si>
+  <si>
+    <t>First check if GCD is possible with str1 + str2 == str2 + str1. We use the Euclidean algorithm to recursively find the substring.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/greatest-common-divisor-of-strings/solutions/3124997/super-easy-solution-fully-explained-c-python3-java/?envType=study-plan-v2&amp;envId=leetcode-75</t>
+  </si>
+  <si>
+    <t>605. Can Place Flowers</t>
+  </si>
+  <si>
+    <t>The Optimal solution is the Greedy solution. Greedily place a flower at every vacant spot from left to right. The Naïve solution is that you can do a for loop, checking each triplet if they are all 0's, and handle th edge cases (n=0, l=1, l=2, starting i and ending i. Increment a count.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/can-place-flowers/solutions/103898/java-greedy-solution-o-flowerbed-beats-100/?envType=study-plan-v2&amp;envId=leetcode-75 </t>
   </si>
 </sst>
 </file>
@@ -816,10 +834,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1508,6 +1526,40 @@
       </c>
       <c r="E40" s="2" t="s">
         <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>143</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" t="s">
+        <v>140</v>
+      </c>
+      <c r="D41" t="s">
+        <v>144</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>146</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" t="s">
+        <v>147</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1551,6 +1603,8 @@
     <hyperlink ref="E38" r:id="rId37" xr:uid="{E8445F29-8F3E-469F-8E84-916FDFC5CB09}"/>
     <hyperlink ref="E39" r:id="rId38" xr:uid="{88D49C5D-6104-4B6C-9B91-ED5642D8BF91}"/>
     <hyperlink ref="E40" r:id="rId39" xr:uid="{8A18F5D6-4553-453B-800F-B5523B2CD512}"/>
+    <hyperlink ref="E41" r:id="rId40" xr:uid="{0B83878A-FA4D-4F2F-845D-8BE73C9984B5}"/>
+    <hyperlink ref="E42" r:id="rId41" xr:uid="{AA2A8642-66CC-40F2-9D86-3ADA93EAF544}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dsa greedy and web
</commit_message>
<xml_diff>
--- a/java/TopInterview150_LC75.xlsx
+++ b/java/TopInterview150_LC75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0157FB-7B21-4595-B5FD-FC5E87ACFE5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033915BF-88CE-42F8-9B08-C142806AB2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="152">
   <si>
     <t>Question</t>
   </si>
@@ -483,6 +483,15 @@
   </si>
   <si>
     <t xml:space="preserve">https://leetcode.com/problems/can-place-flowers/solutions/103898/java-greedy-solution-o-flowerbed-beats-100/?envType=study-plan-v2&amp;envId=leetcode-75 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/best-time-to-buy-and-sell-stock-ii/solutions/208241/explanation-for-the-dummy-like-me/?envType=study-plan-v2&amp;envId=top-interview-150 </t>
+  </si>
+  <si>
+    <t>122. Best Time to Buy and Sell Stock II</t>
+  </si>
+  <si>
+    <t>The crux is that we solve this with a greedy approach. It is always better to buy local minima and sell at the next local high, rather than buy at the global minimum and sell at the global maximum. Use a while loop i &lt; n, and 2 inner while loops for buy and sell, using prices[i+1] to search for conditions.</t>
   </si>
 </sst>
 </file>
@@ -834,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,6 +1569,23 @@
       </c>
       <c r="E42" s="2" t="s">
         <v>148</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>150</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" t="s">
+        <v>151</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1605,6 +1631,7 @@
     <hyperlink ref="E40" r:id="rId39" xr:uid="{8A18F5D6-4553-453B-800F-B5523B2CD512}"/>
     <hyperlink ref="E41" r:id="rId40" xr:uid="{0B83878A-FA4D-4F2F-845D-8BE73C9984B5}"/>
     <hyperlink ref="E42" r:id="rId41" xr:uid="{AA2A8642-66CC-40F2-9D86-3ADA93EAF544}"/>
+    <hyperlink ref="E43" r:id="rId42" xr:uid="{7C169B9E-58F8-43A2-959F-B6D69C630A08}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dsa hashing and web quiz
</commit_message>
<xml_diff>
--- a/java/TopInterview150_LC75.xlsx
+++ b/java/TopInterview150_LC75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC808CD-24BA-4D43-9638-4BE982FA9321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AEC886-280B-42A0-A0EE-29A7EE240E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="182">
   <si>
     <t>Question</t>
   </si>
@@ -573,6 +573,15 @@
   </si>
   <si>
     <t>Classic Sliding Window. With only 1 deletion, we only need to count the first deletion, then greedily move until the next 0 is encountered, compute max window, then move the left pointer past the last 0. If deletion was not used at all, return nums.length - 1. It can be very clean.</t>
+  </si>
+  <si>
+    <t>1657. Determine If Two Strings Are Close</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/determine-if-two-strings-are-close/solutions/4561223/beats-99-46-users-c-java-python-javascript-explained/?envType=study-plan-v2&amp;envId=leetcode-75 </t>
+  </si>
+  <si>
+    <t>The crux is to understand the permutation and combination principle. The order does not matter, only if the set of items and their frequencies matter. You take counters of counters, or buckets. Collect the frequencies in maps, check if they have the same characters, and then check if the frequencies are equal. It is easiest to sort after the char check, then do a freq check. You can return freq1 == freq2 after sort.</t>
   </si>
 </sst>
 </file>
@@ -924,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1820,6 +1829,23 @@
       </c>
       <c r="E52" s="2" t="s">
         <v>177</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>179</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" t="s">
+        <v>22</v>
+      </c>
+      <c r="D53" t="s">
+        <v>181</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -1875,6 +1901,7 @@
     <hyperlink ref="E50" r:id="rId49" xr:uid="{103E5860-844D-48D9-8919-4722FCFCD75C}"/>
     <hyperlink ref="E51" r:id="rId50" xr:uid="{7597B714-A15D-4B6D-8B51-FA22A867FA42}"/>
     <hyperlink ref="E52" r:id="rId51" xr:uid="{89A26D84-0FC0-4582-9CA2-22A0A414EF61}"/>
+    <hyperlink ref="E53" r:id="rId52" xr:uid="{1AA56464-3EB4-40DB-B7F9-FB6333C21FF7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dsa queues and sql
</commit_message>
<xml_diff>
--- a/java/TopInterview150_LC75.xlsx
+++ b/java/TopInterview150_LC75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F118745-8E41-4B34-A31D-F0AE0A7E875A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B55058-1D25-495B-B7BB-2C4548CBD945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="191">
   <si>
     <t>Question</t>
   </si>
@@ -600,6 +600,15 @@
   </si>
   <si>
     <t>The crux is to use 2 hashmaps, and iterate the columns while iterating rows. You can get the row values with grid[i][j] and col values with grid[j][i]. When you iterate the hashmaps to get the count, you need to get the product of the frequencies, not the sum, as each row can match with each col and vice versa. Optimally, only 1 map is needed.</t>
+  </si>
+  <si>
+    <t>649. Dota2 Senate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/dota2-senate/solutions/3483399/simple-diagram-explanation/?envType=study-plan-v2&amp;envId=leetcode-75 </t>
+  </si>
+  <si>
+    <t>The Optimal solution uses 2 queues and index comparisons. Use a queue, the actions that each node can take is only to add a ban count. Keep track of counts for each type of node and also ban counts. Push back into the q like a BFS if there are no bans in place. Make sure the return condition handles both 1 node remaining and if only 1 team's nodes remain.</t>
   </si>
 </sst>
 </file>
@@ -951,10 +960,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1898,6 +1907,23 @@
       </c>
       <c r="E55" s="2" t="s">
         <v>186</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>188</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56" t="s">
+        <v>84</v>
+      </c>
+      <c r="D56" t="s">
+        <v>190</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -1956,6 +1982,7 @@
     <hyperlink ref="E53" r:id="rId52" xr:uid="{1AA56464-3EB4-40DB-B7F9-FB6333C21FF7}"/>
     <hyperlink ref="E54" r:id="rId53" xr:uid="{0451FD0D-7DD5-4B5A-8894-28670CAD1CD0}"/>
     <hyperlink ref="E55" r:id="rId54" xr:uid="{753208C0-5AB6-4B55-8DF2-8A30426C453E}"/>
+    <hyperlink ref="E56" r:id="rId55" xr:uid="{A199E782-D2B6-4D21-AAC4-57C2D6679DF2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dsa trees and sql joins
</commit_message>
<xml_diff>
--- a/java/TopInterview150_LC75.xlsx
+++ b/java/TopInterview150_LC75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C130FE4D-CB95-4C9F-8EEC-9158CD0758C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6BA686-A68A-44BD-9AD5-C065D1986D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="197">
   <si>
     <t>Question</t>
   </si>
@@ -618,6 +618,15 @@
   </si>
   <si>
     <t>Classic Recursive DFS with O(n^2) worst case O(nlogn) best case in balanced tree Time and O(n) space. Call dfs on the root, left, and right. Dfs should be 1 or 0 + left and right, where the targetSum is targetSum - node.val. Remember to call DFS from the root, but recurse the original function on the left and the right! The optimal solution uses a hashmap for prefix Sum.</t>
+  </si>
+  <si>
+    <t>1372. Longest ZigZag Path in a Binary Tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/longest-zigzag-path-in-a-binary-tree/solutions/531867/java-python-dfs-solution/?envType=study-plan-v2&amp;envId=leetcode-75 </t>
+  </si>
+  <si>
+    <t>For a simple solution, maintain a global max variable. Propagate the depth and the direction. Call the recursive function on both sides at the start, and at each node, check to override max, and then call dfs on both sides once again. If the conditions are maintained, add depth+1, else reset depth to 0.</t>
   </si>
 </sst>
 </file>
@@ -969,10 +978,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1950,6 +1959,23 @@
       </c>
       <c r="E57" s="2" t="s">
         <v>192</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>194</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58" t="s">
+        <v>28</v>
+      </c>
+      <c r="D58" t="s">
+        <v>196</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -2010,6 +2036,7 @@
     <hyperlink ref="E55" r:id="rId54" xr:uid="{753208C0-5AB6-4B55-8DF2-8A30426C453E}"/>
     <hyperlink ref="E56" r:id="rId55" xr:uid="{A199E782-D2B6-4D21-AAC4-57C2D6679DF2}"/>
     <hyperlink ref="E57" r:id="rId56" xr:uid="{D5D439A2-CA88-48FA-A484-7A88078CCCCA}"/>
+    <hyperlink ref="E58" r:id="rId57" xr:uid="{806DFEF8-9220-4619-B876-7F7D95F341D9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dsa heaps, sql, python
</commit_message>
<xml_diff>
--- a/java/TopInterview150_LC75.xlsx
+++ b/java/TopInterview150_LC75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8C7444-A1D4-4972-8965-86A795B991EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D222E3-DCA9-4A95-86BF-47265C58DB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="218">
   <si>
     <t>Question</t>
   </si>
@@ -681,6 +681,15 @@
   </si>
   <si>
     <t xml:space="preserve">https://leetcode.com/problems/nearest-exit-from-entrance-in-maze/solutions/2834640/java-explained-in-detail-simple-fast-solution-bfs/?envType=study-plan-v2&amp;envId=leetcode-75 </t>
+  </si>
+  <si>
+    <t>2542. Maximum Subsequence Score</t>
+  </si>
+  <si>
+    <t>The crux is that we consider for each element of nums2[i] as aminimum once and check for max possible values in num1. We first sort nums2 and keep their mappings to nums1, then iterate the pairs maintaing a heap with size k. First form the pairs as int[][]. Iterate the pairs and sort with nums2 from large to small. Keep a priority queue of size k. Each time we introduce a new pair, maintain the min value of nums2 and the sum of the priority queue. If the size of the q &gt; k, pop min nums1, update sum -= nums1. If the size of q = k, update res = max(res, sum * nums2[i]).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/maximum-subsequence-score/solutions/3557445/java-solution-for-maximum-subsequence-score-problem/?envType=study-plan-v2&amp;envId=leetcode-75 </t>
   </si>
 </sst>
 </file>
@@ -1032,10 +1041,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2132,6 +2141,23 @@
       </c>
       <c r="E64" s="2" t="s">
         <v>214</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>215</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C65" t="s">
+        <v>136</v>
+      </c>
+      <c r="D65" t="s">
+        <v>216</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -2199,6 +2225,7 @@
     <hyperlink ref="E62" r:id="rId61" xr:uid="{30E93616-66A2-4508-A954-C3165AF089F1}"/>
     <hyperlink ref="E63" r:id="rId62" xr:uid="{C64C9BC2-DCCC-40FD-B3F9-12E02648A555}"/>
     <hyperlink ref="E64" r:id="rId63" xr:uid="{C5F5F780-6180-436D-9891-954235937689}"/>
+    <hyperlink ref="E65" r:id="rId64" xr:uid="{9AB3AAD1-8E87-4A9F-9180-7469A4398142}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dsa binary search, python, sql
</commit_message>
<xml_diff>
--- a/java/TopInterview150_LC75.xlsx
+++ b/java/TopInterview150_LC75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3064606-5A95-4132-9CDF-A093051AED91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95512B79-9218-419A-8A19-66ECFE584618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="224">
   <si>
     <t>Question</t>
   </si>
@@ -699,6 +699,15 @@
   </si>
   <si>
     <t>Maintain 2 priority queues for beginning and end of the list. And at each iteration, compare tops, then poll the smallest and add to cost.</t>
+  </si>
+  <si>
+    <t>2300. Successful Pairs of Spells and Potions</t>
+  </si>
+  <si>
+    <t>First sort the pairs array. For loop over all spells and do a binary search to find the first mid point which results in a success. Because we previously sorted potions, all indices after that are valid, so add that count to the pairs[i].</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/successful-pairs-of-spells-and-potions/solutions/3367914/easy-solutions-in-java-python-and-c-look-at-once-with-exaplanation/?envType=study-plan-v2&amp;envId=leetcode-75 </t>
   </si>
 </sst>
 </file>
@@ -1050,10 +1059,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B49" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2184,6 +2193,23 @@
       </c>
       <c r="E66" s="2" t="s">
         <v>219</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>221</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67" t="s">
+        <v>52</v>
+      </c>
+      <c r="D67" t="s">
+        <v>222</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -2253,6 +2279,7 @@
     <hyperlink ref="E64" r:id="rId63" xr:uid="{C5F5F780-6180-436D-9891-954235937689}"/>
     <hyperlink ref="E65" r:id="rId64" xr:uid="{9AB3AAD1-8E87-4A9F-9180-7469A4398142}"/>
     <hyperlink ref="E66" r:id="rId65" xr:uid="{9407C8FF-D01E-4A71-80E5-FA995D2E406B}"/>
+    <hyperlink ref="E67" r:id="rId66" xr:uid="{62AF6134-C934-4549-94A3-4140D55A977D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dsa stacks, python, sql
</commit_message>
<xml_diff>
--- a/java/TopInterview150_LC75.xlsx
+++ b/java/TopInterview150_LC75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8580A707-8D27-4582-BCE4-9C3E0F02CC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3532215-A5A1-4710-9F4D-94A100C6901E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="233">
   <si>
     <t>Question</t>
   </si>
@@ -726,6 +726,15 @@
   </si>
   <si>
     <t>A Fibonacci variation. The crux is to recognize the 6 types of shapes that can be made (using rotation), and the reccurrence relation of p1 * 2L + p3.</t>
+  </si>
+  <si>
+    <t>901. Online Stock Span</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/online-stock-span/solutions/168311/c-java-python-o-1/?envType=study-plan-v2&amp;envId=leetcode-75 </t>
+  </si>
+  <si>
+    <t>Push every pair of &lt;price, result&gt; to a stack. Pop the lower price from the stack and accumulate the count. We can keep popping from the stack when we call next() because we store the result at the time of pushing each element. Thus we maintain the stack invariant and we effectively collapse the spans into a single value.</t>
   </si>
 </sst>
 </file>
@@ -1077,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2262,6 +2271,23 @@
       </c>
       <c r="E69" s="2" t="s">
         <v>227</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>230</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C70" t="s">
+        <v>74</v>
+      </c>
+      <c r="D70" t="s">
+        <v>232</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -2334,6 +2360,7 @@
     <hyperlink ref="E67" r:id="rId66" xr:uid="{62AF6134-C934-4549-94A3-4140D55A977D}"/>
     <hyperlink ref="E68" r:id="rId67" xr:uid="{88BC1F2C-5394-48C4-BF37-1F8638C0293B}"/>
     <hyperlink ref="E69" r:id="rId68" xr:uid="{C7D53A05-8133-46FB-977F-BBA942491A8B}"/>
+    <hyperlink ref="E70" r:id="rId69" xr:uid="{E80080A9-9E57-41D5-90B3-42F166588DED}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dsa intervals, python, sql, web landing page
</commit_message>
<xml_diff>
--- a/java/TopInterview150_LC75.xlsx
+++ b/java/TopInterview150_LC75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3532215-A5A1-4710-9F4D-94A100C6901E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0500BE37-ED9B-4793-958E-B9D13512EF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="236">
   <si>
     <t>Question</t>
   </si>
@@ -735,6 +735,15 @@
   </si>
   <si>
     <t>Push every pair of &lt;price, result&gt; to a stack. Pop the lower price from the stack and accumulate the count. We can keep popping from the stack when we call next() because we store the result at the time of pushing each element. Thus we maintain the stack invariant and we effectively collapse the spans into a single value.</t>
+  </si>
+  <si>
+    <t>452. Minimum Number of Arrows to Burst Balloons</t>
+  </si>
+  <si>
+    <t>Greedy approach. First sort the balloons by their ending position with Integer.compare(a[1],b[1]), then iterate, shooting the arrow at the ending position of the current balloon, then start again from the next one. You iterate by points[i][1] and set the arrow there, then check if points[i][0] falls in that range. If it is, you continue without iterating arrow count or shifting the arrow position. For large values, you have to use Integer compare, or convert to long first.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons/solutions/1686627/c-java-python-6-lines-sort-and-greedy-image-explanation/?envType=study-plan-v2&amp;envId=leetcode-75 </t>
   </si>
 </sst>
 </file>
@@ -1086,10 +1095,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2288,6 +2297,23 @@
       </c>
       <c r="E70" s="2" t="s">
         <v>231</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>233</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71" t="s">
+        <v>21</v>
+      </c>
+      <c r="D71" t="s">
+        <v>234</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -2361,6 +2387,7 @@
     <hyperlink ref="E68" r:id="rId67" xr:uid="{88BC1F2C-5394-48C4-BF37-1F8638C0293B}"/>
     <hyperlink ref="E69" r:id="rId68" xr:uid="{C7D53A05-8133-46FB-977F-BBA942491A8B}"/>
     <hyperlink ref="E70" r:id="rId69" xr:uid="{E80080A9-9E57-41D5-90B3-42F166588DED}"/>
+    <hyperlink ref="E71" r:id="rId70" xr:uid="{8C578E30-08C8-4B95-AFDC-D0F8BB8A8D31}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dsa tries and bits
</commit_message>
<xml_diff>
--- a/java/TopInterview150_LC75.xlsx
+++ b/java/TopInterview150_LC75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0500BE37-ED9B-4793-958E-B9D13512EF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878CDDF1-AC1E-45A5-B5B9-173682BFA38F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="243">
   <si>
     <t>Question</t>
   </si>
@@ -744,6 +744,27 @@
   </si>
   <si>
     <t xml:space="preserve">https://leetcode.com/problems/minimum-number-of-arrows-to-burst-balloons/solutions/1686627/c-java-python-6-lines-sort-and-greedy-image-explanation/?envType=study-plan-v2&amp;envId=leetcode-75 </t>
+  </si>
+  <si>
+    <t>1268. Search Suggestions System</t>
+  </si>
+  <si>
+    <t>Tries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/search-suggestions-system/solutions/436151/java-python-3-simple-trie-and-binary-search-codes-w-comment-and-brief-analysis/?envType=study-plan-v2&amp;envId=leetcode-75 </t>
+  </si>
+  <si>
+    <t>Classic Trie, but can be solved with Binary Search. Use DS principles. Class Trie with linked list for suggestions.</t>
+  </si>
+  <si>
+    <t>1318. Minimum Flips to Make a OR b Equal to c</t>
+  </si>
+  <si>
+    <t>Quick trick is use Integer.bitCount(), but from first principles, use a bit mask.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/minimum-flips-to-make-a-or-b-equal-to-c/solutions/477690/java-python-3-bit-manipulation-w-explanation-and-analysis/?envType=study-plan-v2&amp;envId=leetcode-75 </t>
   </si>
 </sst>
 </file>
@@ -1095,10 +1116,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+      <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2314,6 +2335,40 @@
       </c>
       <c r="E71" s="2" t="s">
         <v>235</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>236</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72" t="s">
+        <v>237</v>
+      </c>
+      <c r="D72" t="s">
+        <v>239</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>240</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73" t="s">
+        <v>35</v>
+      </c>
+      <c r="D73" t="s">
+        <v>241</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -2388,6 +2443,8 @@
     <hyperlink ref="E69" r:id="rId68" xr:uid="{C7D53A05-8133-46FB-977F-BBA942491A8B}"/>
     <hyperlink ref="E70" r:id="rId69" xr:uid="{E80080A9-9E57-41D5-90B3-42F166588DED}"/>
     <hyperlink ref="E71" r:id="rId70" xr:uid="{8C578E30-08C8-4B95-AFDC-D0F8BB8A8D31}"/>
+    <hyperlink ref="E72" r:id="rId71" xr:uid="{85178379-D2CB-481C-A06D-76A4A23A4AE3}"/>
+    <hyperlink ref="E73" r:id="rId72" xr:uid="{6314FEA8-666D-4BEB-9C8B-470710D2C03C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dsa math and web
</commit_message>
<xml_diff>
--- a/java/TopInterview150_LC75.xlsx
+++ b/java/TopInterview150_LC75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11E81B6-F116-463F-A74C-D0C82F94C788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF544AB-734F-4151-8015-33E39C04CB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="265">
   <si>
     <t>Question</t>
   </si>
@@ -819,6 +819,18 @@
   </si>
   <si>
     <t>We use Kadane's algorithm. The subarray can either be contained in one pass (middle) of the array, in which case we do max subarray, and if the subarray is split left and right, we use Kadane's to find the max subarray sum. We can subtract the minimum subarray sum from the total to get it.</t>
+  </si>
+  <si>
+    <t>172. Factorial Trailing Zeroes</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/factorial-trailing-zeroes/solutions/52371/my-one-line-solutions-in-3-languages/comments/53281 </t>
+  </si>
+  <si>
+    <t>The crux is we just count how many 5 factors in all number from 1 to n.</t>
   </si>
 </sst>
 </file>
@@ -1170,10 +1182,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B55" workbookViewId="0">
-      <selection activeCell="E83" sqref="E83"/>
+      <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2525,6 +2537,23 @@
       </c>
       <c r="E79" s="2" t="s">
         <v>259</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>261</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C80" t="s">
+        <v>262</v>
+      </c>
+      <c r="D80" t="s">
+        <v>264</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -2607,6 +2636,7 @@
     <hyperlink ref="E77" r:id="rId76" xr:uid="{3C9FF9EA-3484-4DF7-9BAA-3AF06CB94C37}"/>
     <hyperlink ref="E78" r:id="rId77" xr:uid="{9E727E47-93A4-473A-8D42-19323A09A444}"/>
     <hyperlink ref="E79" r:id="rId78" xr:uid="{4106909D-2B79-401B-9819-79322EFD5057}"/>
+    <hyperlink ref="E80" r:id="rId79" xr:uid="{4223715A-41DE-418D-B692-8965F343C12D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dsa arrays and math
</commit_message>
<xml_diff>
--- a/java/TopInterview150_LC75.xlsx
+++ b/java/TopInterview150_LC75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D6BDFF-7515-4C9A-91DB-0861C7979FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8070E8D1-48CE-4A7C-AC6F-F321582F164F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="286">
   <si>
     <t>Question</t>
   </si>
@@ -876,6 +876,24 @@
   </si>
   <si>
     <t>We need to keep collecting characters from the original string to corresponding Strings in a String array. Keep track of indices i and j to keep them in bound.</t>
+  </si>
+  <si>
+    <t>28. Find the Index of the First Occurrence in a String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We can use a 2d for loop to iterate the haystack's chars and needle's chars. If i + needle length &gt; haystack length, immediately break, iterate if haystack.charAt(i+j) is equal to needle.charAt(j) and iterate until j == needle length. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/find-the-index-of-the-first-occurrence-in-a-string/solutions/12807/elegant-java-solution/comments/142986 </t>
+  </si>
+  <si>
+    <t>69. Sqrt(x)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/sqrtx/solutions/25057/3-4-short-lines-integer-newton-every-language/?envType=study-plan-v2&amp;envId=top-interview-150 </t>
+  </si>
+  <si>
+    <t>Optimally, use the Newton method. Otherwise, use binary search with the search condition of the square of mid &gt; mid.</t>
   </si>
 </sst>
 </file>
@@ -1227,10 +1245,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B61" workbookViewId="0">
-      <selection activeCell="E88" sqref="E88"/>
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2684,6 +2702,40 @@
       </c>
       <c r="E85" s="2" t="s">
         <v>278</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>280</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C86" t="s">
+        <v>17</v>
+      </c>
+      <c r="D86" t="s">
+        <v>281</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>283</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C87" t="s">
+        <v>262</v>
+      </c>
+      <c r="D87" t="s">
+        <v>285</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -2772,6 +2824,8 @@
     <hyperlink ref="E83" r:id="rId82" xr:uid="{3129A68B-0F69-4729-96C5-F4B919F28418}"/>
     <hyperlink ref="E84" r:id="rId83" xr:uid="{39AED362-27A0-4FCD-BAE5-38827A94121A}"/>
     <hyperlink ref="E85" r:id="rId84" xr:uid="{2D61FCFC-CFF4-4B66-AA9A-D75B6D60EC6C}"/>
+    <hyperlink ref="E86" r:id="rId85" xr:uid="{C7DD88AF-1EB3-4BEF-B67E-186218492428}"/>
+    <hyperlink ref="E87" r:id="rId86" xr:uid="{FE6EA361-3CEB-4641-B3D5-30D1B3D97004}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>